<commit_message>
Add seq id to fieldsample_barcode map
</commit_message>
<xml_diff>
--- a/analysis/mails_01/P10_2/table_to_fill.xlsx
+++ b/analysis/mails_01/P10_2/table_to_fill.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="584">
   <si>
     <t xml:space="preserve">fieldsample_barcode</t>
   </si>
@@ -388,15 +388,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gudenå</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MFD00228</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56.8255986</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.8112735</t>
   </si>
   <si>
     <t xml:space="preserve">MFD01464</t>
@@ -3225,13 +3216,13 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F27" t="s">
         <v>19</v>
@@ -3240,7 +3231,7 @@
         <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="I27" t="s">
         <v>22</v>
@@ -3261,19 +3252,19 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E28" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -3282,7 +3273,7 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I28" t="s">
         <v>22</v>
@@ -3303,19 +3294,19 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E29" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F29" t="s">
         <v>19</v>
@@ -3324,7 +3315,7 @@
         <v>20</v>
       </c>
       <c r="H29" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I29" t="s">
         <v>22</v>
@@ -3345,19 +3336,19 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E30" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F30" t="s">
         <v>19</v>
@@ -3366,7 +3357,7 @@
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="I30" t="s">
         <v>22</v>
@@ -3387,13 +3378,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D31" t="s">
         <v>145</v>
@@ -3408,7 +3399,7 @@
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I31" t="s">
         <v>22</v>
@@ -3435,7 +3426,7 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D32" t="s">
         <v>148</v>
@@ -3450,7 +3441,7 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="I32" t="s">
         <v>22</v>
@@ -3471,19 +3462,19 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="D33" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F33" t="s">
         <v>19</v>
@@ -3492,7 +3483,7 @@
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I33" t="s">
         <v>22</v>
@@ -3513,19 +3504,19 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E34" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
@@ -3534,7 +3525,7 @@
         <v>20</v>
       </c>
       <c r="H34" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I34" t="s">
         <v>22</v>
@@ -3555,19 +3546,19 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E35" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F35" t="s">
         <v>19</v>
@@ -3576,7 +3567,7 @@
         <v>20</v>
       </c>
       <c r="H35" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I35" t="s">
         <v>22</v>
@@ -3597,19 +3588,19 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B36" t="s">
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D36" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E36" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
@@ -3618,7 +3609,7 @@
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I36" t="s">
         <v>22</v>
@@ -3639,19 +3630,19 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B37" t="s">
         <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D37" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E37" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F37" t="s">
         <v>19</v>
@@ -3660,7 +3651,7 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I37" t="s">
         <v>22</v>
@@ -3681,19 +3672,19 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="D38" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E38" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F38" t="s">
         <v>19</v>
@@ -3702,7 +3693,7 @@
         <v>20</v>
       </c>
       <c r="H38" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I38" t="s">
         <v>22</v>
@@ -3723,19 +3714,19 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="D39" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E39" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F39" t="s">
         <v>19</v>
@@ -3744,7 +3735,7 @@
         <v>20</v>
       </c>
       <c r="H39" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I39" t="s">
         <v>22</v>
@@ -3765,19 +3756,19 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B40" t="s">
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D40" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E40" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F40" t="s">
         <v>19</v>
@@ -3786,7 +3777,7 @@
         <v>20</v>
       </c>
       <c r="H40" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I40" t="s">
         <v>22</v>
@@ -3807,19 +3798,19 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E41" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F41" t="s">
         <v>19</v>
@@ -3828,7 +3819,7 @@
         <v>20</v>
       </c>
       <c r="H41" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I41" t="s">
         <v>22</v>
@@ -3849,19 +3840,19 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B42" t="s">
         <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="D42" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E42" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F42" t="s">
         <v>19</v>
@@ -3870,7 +3861,7 @@
         <v>20</v>
       </c>
       <c r="H42" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I42" t="s">
         <v>22</v>
@@ -3891,19 +3882,19 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B43" t="s">
         <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D43" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E43" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F43" t="s">
         <v>19</v>
@@ -3912,7 +3903,7 @@
         <v>20</v>
       </c>
       <c r="H43" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I43" t="s">
         <v>22</v>
@@ -3933,19 +3924,19 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D44" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E44" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F44" t="s">
         <v>19</v>
@@ -3954,7 +3945,7 @@
         <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I44" t="s">
         <v>22</v>
@@ -3975,19 +3966,19 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="D45" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E45" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F45" t="s">
         <v>19</v>
@@ -3996,7 +3987,7 @@
         <v>20</v>
       </c>
       <c r="H45" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I45" t="s">
         <v>22</v>
@@ -4017,19 +4008,19 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B46" t="s">
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E46" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F46" t="s">
         <v>19</v>
@@ -4038,7 +4029,7 @@
         <v>20</v>
       </c>
       <c r="H46" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I46" t="s">
         <v>22</v>
@@ -4059,19 +4050,19 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B47" t="s">
         <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="D47" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E47" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F47" t="s">
         <v>19</v>
@@ -4080,7 +4071,7 @@
         <v>20</v>
       </c>
       <c r="H47" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="I47" t="s">
         <v>22</v>
@@ -4107,13 +4098,13 @@
         <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>218</v>
       </c>
       <c r="D48" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E48" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F48" t="s">
         <v>19</v>
@@ -4122,7 +4113,7 @@
         <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="I48" t="s">
         <v>22</v>
@@ -4143,19 +4134,19 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B49" t="s">
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="D49" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E49" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F49" t="s">
         <v>19</v>
@@ -4164,7 +4155,7 @@
         <v>20</v>
       </c>
       <c r="H49" t="s">
-        <v>224</v>
+        <v>124</v>
       </c>
       <c r="I49" t="s">
         <v>22</v>
@@ -4191,13 +4182,13 @@
         <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="D50" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E50" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F50" t="s">
         <v>19</v>
@@ -4206,7 +4197,7 @@
         <v>20</v>
       </c>
       <c r="H50" t="s">
-        <v>124</v>
+        <v>229</v>
       </c>
       <c r="I50" t="s">
         <v>22</v>
@@ -4227,19 +4218,19 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B51" t="s">
         <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>229</v>
+        <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E51" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F51" t="s">
         <v>19</v>
@@ -4248,7 +4239,7 @@
         <v>20</v>
       </c>
       <c r="H51" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I51" t="s">
         <v>22</v>
@@ -4269,19 +4260,19 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B52" t="s">
         <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>235</v>
       </c>
       <c r="D52" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E52" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F52" t="s">
         <v>19</v>
@@ -4290,7 +4281,7 @@
         <v>20</v>
       </c>
       <c r="H52" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I52" t="s">
         <v>22</v>
@@ -4311,19 +4302,19 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B53" t="s">
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>238</v>
+        <v>152</v>
       </c>
       <c r="D53" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E53" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F53" t="s">
         <v>19</v>
@@ -4332,7 +4323,7 @@
         <v>20</v>
       </c>
       <c r="H53" t="s">
-        <v>241</v>
+        <v>168</v>
       </c>
       <c r="I53" t="s">
         <v>22</v>
@@ -4359,7 +4350,7 @@
         <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D54" t="s">
         <v>243</v>
@@ -4374,7 +4365,7 @@
         <v>20</v>
       </c>
       <c r="H54" t="s">
-        <v>171</v>
+        <v>245</v>
       </c>
       <c r="I54" t="s">
         <v>22</v>
@@ -4395,19 +4386,19 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D55" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E55" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F55" t="s">
         <v>19</v>
@@ -4416,7 +4407,7 @@
         <v>20</v>
       </c>
       <c r="H55" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="I55" t="s">
         <v>22</v>
@@ -4437,19 +4428,19 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B56" t="s">
         <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="D56" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E56" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F56" t="s">
         <v>19</v>
@@ -4458,7 +4449,7 @@
         <v>20</v>
       </c>
       <c r="H56" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I56" t="s">
         <v>22</v>
@@ -4479,19 +4470,19 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>229</v>
+        <v>170</v>
       </c>
       <c r="D57" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E57" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F57" t="s">
         <v>19</v>
@@ -4500,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="H57" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I57" t="s">
         <v>22</v>
@@ -4521,19 +4512,19 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>173</v>
+        <v>226</v>
       </c>
       <c r="D58" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E58" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F58" t="s">
         <v>19</v>
@@ -4542,7 +4533,7 @@
         <v>20</v>
       </c>
       <c r="H58" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I58" t="s">
         <v>22</v>
@@ -4563,19 +4554,19 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
       </c>
       <c r="C59" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="D59" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E59" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F59" t="s">
         <v>19</v>
@@ -4584,7 +4575,7 @@
         <v>20</v>
       </c>
       <c r="H59" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I59" t="s">
         <v>22</v>
@@ -4605,19 +4596,19 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D60" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E60" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F60" t="s">
         <v>19</v>
@@ -4626,7 +4617,7 @@
         <v>20</v>
       </c>
       <c r="H60" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I60" t="s">
         <v>22</v>
@@ -4647,19 +4638,19 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>229</v>
+        <v>170</v>
       </c>
       <c r="D61" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E61" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F61" t="s">
         <v>19</v>
@@ -4668,7 +4659,7 @@
         <v>20</v>
       </c>
       <c r="H61" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="I61" t="s">
         <v>22</v>
@@ -4695,13 +4686,13 @@
         <v>15</v>
       </c>
       <c r="C62" t="s">
-        <v>173</v>
+        <v>274</v>
       </c>
       <c r="D62" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E62" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F62" t="s">
         <v>19</v>
@@ -4710,7 +4701,7 @@
         <v>20</v>
       </c>
       <c r="H62" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="I62" t="s">
         <v>22</v>
@@ -4731,19 +4722,19 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B63" t="s">
         <v>15</v>
       </c>
       <c r="C63" t="s">
-        <v>277</v>
+        <v>179</v>
       </c>
       <c r="D63" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E63" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F63" t="s">
         <v>19</v>
@@ -4752,7 +4743,7 @@
         <v>20</v>
       </c>
       <c r="H63" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="I63" t="s">
         <v>22</v>
@@ -4779,7 +4770,7 @@
         <v>15</v>
       </c>
       <c r="C64" t="s">
-        <v>182</v>
+        <v>274</v>
       </c>
       <c r="D64" t="s">
         <v>282</v>
@@ -4794,7 +4785,7 @@
         <v>20</v>
       </c>
       <c r="H64" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
       <c r="I64" t="s">
         <v>22</v>
@@ -4815,19 +4806,19 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B65" t="s">
         <v>15</v>
       </c>
       <c r="C65" t="s">
-        <v>277</v>
+        <v>235</v>
       </c>
       <c r="D65" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E65" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F65" t="s">
         <v>19</v>
@@ -4836,7 +4827,7 @@
         <v>20</v>
       </c>
       <c r="H65" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I65" t="s">
         <v>22</v>
@@ -4857,19 +4848,19 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B66" t="s">
         <v>15</v>
       </c>
       <c r="C66" t="s">
-        <v>238</v>
+        <v>170</v>
       </c>
       <c r="D66" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E66" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F66" t="s">
         <v>19</v>
@@ -4878,7 +4869,7 @@
         <v>20</v>
       </c>
       <c r="H66" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="I66" t="s">
         <v>22</v>
@@ -4905,7 +4896,7 @@
         <v>15</v>
       </c>
       <c r="C67" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="D67" t="s">
         <v>293</v>
@@ -4920,7 +4911,7 @@
         <v>20</v>
       </c>
       <c r="H67" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="I67" t="s">
         <v>22</v>
@@ -4941,19 +4932,19 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B68" t="s">
         <v>15</v>
       </c>
       <c r="C68" t="s">
-        <v>155</v>
+        <v>297</v>
       </c>
       <c r="D68" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E68" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F68" t="s">
         <v>19</v>
@@ -4962,7 +4953,7 @@
         <v>20</v>
       </c>
       <c r="H68" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="I68" t="s">
         <v>22</v>
@@ -4983,19 +4974,19 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B69" t="s">
         <v>15</v>
       </c>
       <c r="C69" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D69" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E69" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F69" t="s">
         <v>19</v>
@@ -5004,7 +4995,7 @@
         <v>20</v>
       </c>
       <c r="H69" t="s">
-        <v>303</v>
+        <v>124</v>
       </c>
       <c r="I69" t="s">
         <v>22</v>
@@ -5025,19 +5016,19 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B70" t="s">
         <v>15</v>
       </c>
       <c r="C70" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D70" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E70" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F70" t="s">
         <v>19</v>
@@ -5046,7 +5037,7 @@
         <v>20</v>
       </c>
       <c r="H70" t="s">
-        <v>124</v>
+        <v>309</v>
       </c>
       <c r="I70" t="s">
         <v>22</v>
@@ -5067,19 +5058,19 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B71" t="s">
         <v>15</v>
       </c>
       <c r="C71" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="D71" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E71" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F71" t="s">
         <v>19</v>
@@ -5088,7 +5079,7 @@
         <v>20</v>
       </c>
       <c r="H71" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="I71" t="s">
         <v>22</v>
@@ -5109,19 +5100,19 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B72" t="s">
         <v>15</v>
       </c>
       <c r="C72" t="s">
-        <v>305</v>
+        <v>157</v>
       </c>
       <c r="D72" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E72" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F72" t="s">
         <v>19</v>
@@ -5130,7 +5121,7 @@
         <v>20</v>
       </c>
       <c r="H72" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="I72" t="s">
         <v>22</v>
@@ -5151,19 +5142,19 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B73" t="s">
         <v>15</v>
       </c>
       <c r="C73" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="D73" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E73" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F73" t="s">
         <v>19</v>
@@ -5172,7 +5163,7 @@
         <v>20</v>
       </c>
       <c r="H73" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="I73" t="s">
         <v>22</v>
@@ -5193,19 +5184,19 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B74" t="s">
         <v>15</v>
       </c>
       <c r="C74" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="D74" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E74" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F74" t="s">
         <v>19</v>
@@ -5214,7 +5205,7 @@
         <v>20</v>
       </c>
       <c r="H74" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="I74" t="s">
         <v>22</v>
@@ -5235,19 +5226,19 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B75" t="s">
         <v>15</v>
       </c>
       <c r="C75" t="s">
-        <v>229</v>
+        <v>297</v>
       </c>
       <c r="D75" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E75" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F75" t="s">
         <v>19</v>
@@ -5256,7 +5247,7 @@
         <v>20</v>
       </c>
       <c r="H75" t="s">
-        <v>328</v>
+        <v>300</v>
       </c>
       <c r="I75" t="s">
         <v>22</v>
@@ -5283,7 +5274,7 @@
         <v>15</v>
       </c>
       <c r="C76" t="s">
-        <v>300</v>
+        <v>206</v>
       </c>
       <c r="D76" t="s">
         <v>330</v>
@@ -5298,7 +5289,7 @@
         <v>20</v>
       </c>
       <c r="H76" t="s">
-        <v>303</v>
+        <v>332</v>
       </c>
       <c r="I76" t="s">
         <v>22</v>
@@ -5319,19 +5310,19 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B77" t="s">
         <v>15</v>
       </c>
       <c r="C77" t="s">
-        <v>209</v>
+        <v>306</v>
       </c>
       <c r="D77" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E77" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F77" t="s">
         <v>19</v>
@@ -5340,7 +5331,7 @@
         <v>20</v>
       </c>
       <c r="H77" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="I77" t="s">
         <v>22</v>
@@ -5361,19 +5352,19 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B78" t="s">
         <v>15</v>
       </c>
       <c r="C78" t="s">
-        <v>309</v>
+        <v>206</v>
       </c>
       <c r="D78" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E78" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F78" t="s">
         <v>19</v>
@@ -5382,7 +5373,7 @@
         <v>20</v>
       </c>
       <c r="H78" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="I78" t="s">
         <v>22</v>
@@ -5403,19 +5394,19 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B79" t="s">
         <v>15</v>
       </c>
       <c r="C79" t="s">
-        <v>209</v>
+        <v>274</v>
       </c>
       <c r="D79" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E79" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F79" t="s">
         <v>19</v>
@@ -5424,7 +5415,7 @@
         <v>20</v>
       </c>
       <c r="H79" t="s">
-        <v>343</v>
+        <v>257</v>
       </c>
       <c r="I79" t="s">
         <v>22</v>
@@ -5451,7 +5442,7 @@
         <v>15</v>
       </c>
       <c r="C80" t="s">
-        <v>277</v>
+        <v>179</v>
       </c>
       <c r="D80" t="s">
         <v>345</v>
@@ -5466,7 +5457,7 @@
         <v>20</v>
       </c>
       <c r="H80" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="I80" t="s">
         <v>22</v>
@@ -5493,7 +5484,7 @@
         <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="D81" t="s">
         <v>348</v>
@@ -5508,7 +5499,7 @@
         <v>20</v>
       </c>
       <c r="H81" t="s">
-        <v>252</v>
+        <v>350</v>
       </c>
       <c r="I81" t="s">
         <v>22</v>
@@ -5529,19 +5520,19 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B82" t="s">
         <v>15</v>
       </c>
       <c r="C82" t="s">
-        <v>209</v>
+        <v>152</v>
       </c>
       <c r="D82" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E82" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F82" t="s">
         <v>19</v>
@@ -5550,7 +5541,7 @@
         <v>20</v>
       </c>
       <c r="H82" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="I82" t="s">
         <v>22</v>
@@ -5571,19 +5562,19 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B83" t="s">
         <v>15</v>
       </c>
       <c r="C83" t="s">
-        <v>155</v>
+        <v>297</v>
       </c>
       <c r="D83" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E83" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F83" t="s">
         <v>19</v>
@@ -5592,7 +5583,7 @@
         <v>20</v>
       </c>
       <c r="H83" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="I83" t="s">
         <v>22</v>
@@ -5613,19 +5604,19 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B84" t="s">
         <v>15</v>
       </c>
       <c r="C84" t="s">
-        <v>300</v>
+        <v>152</v>
       </c>
       <c r="D84" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E84" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F84" t="s">
         <v>19</v>
@@ -5634,7 +5625,7 @@
         <v>20</v>
       </c>
       <c r="H84" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="I84" t="s">
         <v>22</v>
@@ -5655,19 +5646,19 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B85" t="s">
         <v>15</v>
       </c>
       <c r="C85" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="D85" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E85" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F85" t="s">
         <v>19</v>
@@ -5676,7 +5667,7 @@
         <v>20</v>
       </c>
       <c r="H85" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="I85" t="s">
         <v>22</v>
@@ -5697,19 +5688,19 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B86" t="s">
         <v>15</v>
       </c>
       <c r="C86" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="D86" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E86" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F86" t="s">
         <v>19</v>
@@ -5718,7 +5709,7 @@
         <v>20</v>
       </c>
       <c r="H86" t="s">
-        <v>369</v>
+        <v>164</v>
       </c>
       <c r="I86" t="s">
         <v>22</v>
@@ -5745,7 +5736,7 @@
         <v>15</v>
       </c>
       <c r="C87" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="D87" t="s">
         <v>371</v>
@@ -5760,7 +5751,7 @@
         <v>20</v>
       </c>
       <c r="H87" t="s">
-        <v>167</v>
+        <v>373</v>
       </c>
       <c r="I87" t="s">
         <v>22</v>
@@ -5781,19 +5772,19 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B88" t="s">
         <v>15</v>
       </c>
       <c r="C88" t="s">
-        <v>134</v>
+        <v>302</v>
       </c>
       <c r="D88" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E88" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F88" t="s">
         <v>19</v>
@@ -5802,7 +5793,7 @@
         <v>20</v>
       </c>
       <c r="H88" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="I88" t="s">
         <v>22</v>
@@ -5823,19 +5814,19 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B89" t="s">
         <v>15</v>
       </c>
       <c r="C89" t="s">
-        <v>305</v>
+        <v>179</v>
       </c>
       <c r="D89" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E89" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F89" t="s">
         <v>19</v>
@@ -5844,7 +5835,7 @@
         <v>20</v>
       </c>
       <c r="H89" t="s">
-        <v>380</v>
+        <v>249</v>
       </c>
       <c r="I89" t="s">
         <v>22</v>
@@ -5871,7 +5862,7 @@
         <v>15</v>
       </c>
       <c r="C90" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="D90" t="s">
         <v>382</v>
@@ -5886,7 +5877,7 @@
         <v>20</v>
       </c>
       <c r="H90" t="s">
-        <v>252</v>
+        <v>124</v>
       </c>
       <c r="I90" t="s">
         <v>22</v>
@@ -5913,7 +5904,7 @@
         <v>15</v>
       </c>
       <c r="C91" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D91" t="s">
         <v>385</v>
@@ -5928,7 +5919,7 @@
         <v>20</v>
       </c>
       <c r="H91" t="s">
-        <v>124</v>
+        <v>387</v>
       </c>
       <c r="I91" t="s">
         <v>22</v>
@@ -5949,19 +5940,19 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B92" t="s">
         <v>15</v>
       </c>
       <c r="C92" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D92" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E92" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F92" t="s">
         <v>19</v>
@@ -5970,7 +5961,7 @@
         <v>20</v>
       </c>
       <c r="H92" t="s">
-        <v>390</v>
+        <v>249</v>
       </c>
       <c r="I92" t="s">
         <v>22</v>
@@ -5997,7 +5988,7 @@
         <v>15</v>
       </c>
       <c r="C93" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="D93" t="s">
         <v>392</v>
@@ -6012,7 +6003,7 @@
         <v>20</v>
       </c>
       <c r="H93" t="s">
-        <v>252</v>
+        <v>394</v>
       </c>
       <c r="I93" t="s">
         <v>22</v>
@@ -6033,19 +6024,19 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B94" t="s">
         <v>15</v>
       </c>
       <c r="C94" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D94" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E94" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F94" t="s">
         <v>19</v>
@@ -6054,7 +6045,7 @@
         <v>20</v>
       </c>
       <c r="H94" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I94" t="s">
         <v>22</v>
@@ -6075,19 +6066,19 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B95" t="s">
         <v>15</v>
       </c>
       <c r="C95" t="s">
-        <v>229</v>
+        <v>152</v>
       </c>
       <c r="D95" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E95" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F95" t="s">
         <v>19</v>
@@ -6096,7 +6087,7 @@
         <v>20</v>
       </c>
       <c r="H95" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I95" t="s">
         <v>22</v>
@@ -6117,19 +6108,19 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B96" t="s">
         <v>15</v>
       </c>
       <c r="C96" t="s">
-        <v>155</v>
+        <v>274</v>
       </c>
       <c r="D96" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E96" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F96" t="s">
         <v>19</v>
@@ -6138,7 +6129,7 @@
         <v>20</v>
       </c>
       <c r="H96" t="s">
-        <v>405</v>
+        <v>284</v>
       </c>
       <c r="I96" t="s">
         <v>22</v>
@@ -6165,7 +6156,7 @@
         <v>15</v>
       </c>
       <c r="C97" t="s">
-        <v>277</v>
+        <v>170</v>
       </c>
       <c r="D97" t="s">
         <v>407</v>
@@ -6180,7 +6171,7 @@
         <v>20</v>
       </c>
       <c r="H97" t="s">
-        <v>287</v>
+        <v>257</v>
       </c>
       <c r="I97" t="s">
         <v>22</v>
@@ -6207,7 +6198,7 @@
         <v>15</v>
       </c>
       <c r="C98" t="s">
-        <v>173</v>
+        <v>302</v>
       </c>
       <c r="D98" t="s">
         <v>410</v>
@@ -6222,7 +6213,7 @@
         <v>20</v>
       </c>
       <c r="H98" t="s">
-        <v>260</v>
+        <v>124</v>
       </c>
       <c r="I98" t="s">
         <v>22</v>
@@ -6249,7 +6240,7 @@
         <v>15</v>
       </c>
       <c r="C99" t="s">
-        <v>305</v>
+        <v>274</v>
       </c>
       <c r="D99" t="s">
         <v>413</v>
@@ -6291,7 +6282,7 @@
         <v>15</v>
       </c>
       <c r="C100" t="s">
-        <v>277</v>
+        <v>206</v>
       </c>
       <c r="D100" t="s">
         <v>416</v>
@@ -6306,7 +6297,7 @@
         <v>20</v>
       </c>
       <c r="H100" t="s">
-        <v>124</v>
+        <v>418</v>
       </c>
       <c r="I100" t="s">
         <v>22</v>
@@ -6327,19 +6318,19 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B101" t="s">
         <v>15</v>
       </c>
       <c r="C101" t="s">
-        <v>209</v>
+        <v>274</v>
       </c>
       <c r="D101" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E101" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F101" t="s">
         <v>19</v>
@@ -6348,7 +6339,7 @@
         <v>20</v>
       </c>
       <c r="H101" t="s">
-        <v>421</v>
+        <v>257</v>
       </c>
       <c r="I101" t="s">
         <v>22</v>
@@ -6375,7 +6366,7 @@
         <v>15</v>
       </c>
       <c r="C102" t="s">
-        <v>277</v>
+        <v>152</v>
       </c>
       <c r="D102" t="s">
         <v>423</v>
@@ -6390,7 +6381,7 @@
         <v>20</v>
       </c>
       <c r="H102" t="s">
-        <v>260</v>
+        <v>425</v>
       </c>
       <c r="I102" t="s">
         <v>22</v>
@@ -6411,19 +6402,19 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B103" t="s">
         <v>15</v>
       </c>
       <c r="C103" t="s">
-        <v>155</v>
+        <v>226</v>
       </c>
       <c r="D103" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E103" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F103" t="s">
         <v>19</v>
@@ -6432,7 +6423,7 @@
         <v>20</v>
       </c>
       <c r="H103" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I103" t="s">
         <v>22</v>
@@ -6453,19 +6444,19 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B104" t="s">
         <v>15</v>
       </c>
       <c r="C104" t="s">
-        <v>229</v>
+        <v>274</v>
       </c>
       <c r="D104" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E104" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F104" t="s">
         <v>19</v>
@@ -6474,7 +6465,7 @@
         <v>20</v>
       </c>
       <c r="H104" t="s">
-        <v>432</v>
+        <v>257</v>
       </c>
       <c r="I104" t="s">
         <v>22</v>
@@ -6501,7 +6492,7 @@
         <v>15</v>
       </c>
       <c r="C105" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D105" t="s">
         <v>434</v>
@@ -6516,7 +6507,7 @@
         <v>20</v>
       </c>
       <c r="H105" t="s">
-        <v>260</v>
+        <v>436</v>
       </c>
       <c r="I105" t="s">
         <v>22</v>
@@ -6537,19 +6528,19 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B106" t="s">
         <v>15</v>
       </c>
       <c r="C106" t="s">
-        <v>277</v>
+        <v>206</v>
       </c>
       <c r="D106" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E106" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F106" t="s">
         <v>19</v>
@@ -6558,7 +6549,7 @@
         <v>20</v>
       </c>
       <c r="H106" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="I106" t="s">
         <v>22</v>
@@ -6579,19 +6570,19 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B107" t="s">
         <v>15</v>
       </c>
       <c r="C107" t="s">
-        <v>209</v>
+        <v>306</v>
       </c>
       <c r="D107" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E107" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="F107" t="s">
         <v>19</v>
@@ -6600,7 +6591,7 @@
         <v>20</v>
       </c>
       <c r="H107" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="I107" t="s">
         <v>22</v>
@@ -6621,19 +6612,19 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B108" t="s">
         <v>15</v>
       </c>
       <c r="C108" t="s">
-        <v>309</v>
+        <v>152</v>
       </c>
       <c r="D108" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E108" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F108" t="s">
         <v>19</v>
@@ -6642,7 +6633,7 @@
         <v>20</v>
       </c>
       <c r="H108" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I108" t="s">
         <v>22</v>
@@ -6663,19 +6654,19 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B109" t="s">
         <v>15</v>
       </c>
       <c r="C109" t="s">
-        <v>155</v>
+        <v>297</v>
       </c>
       <c r="D109" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E109" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F109" t="s">
         <v>19</v>
@@ -6684,7 +6675,7 @@
         <v>20</v>
       </c>
       <c r="H109" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I109" t="s">
         <v>22</v>
@@ -6705,19 +6696,19 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B110" t="s">
         <v>15</v>
       </c>
       <c r="C110" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D110" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E110" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F110" t="s">
         <v>19</v>
@@ -6726,7 +6717,7 @@
         <v>20</v>
       </c>
       <c r="H110" t="s">
-        <v>455</v>
+        <v>124</v>
       </c>
       <c r="I110" t="s">
         <v>22</v>
@@ -6753,7 +6744,7 @@
         <v>15</v>
       </c>
       <c r="C111" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D111" t="s">
         <v>457</v>
@@ -6795,7 +6786,7 @@
         <v>15</v>
       </c>
       <c r="C112" t="s">
-        <v>305</v>
+        <v>226</v>
       </c>
       <c r="D112" t="s">
         <v>460</v>
@@ -6810,7 +6801,7 @@
         <v>20</v>
       </c>
       <c r="H112" t="s">
-        <v>124</v>
+        <v>462</v>
       </c>
       <c r="I112" t="s">
         <v>22</v>
@@ -6831,19 +6822,19 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B113" t="s">
         <v>15</v>
       </c>
       <c r="C113" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D113" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E113" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F113" t="s">
         <v>19</v>
@@ -6852,7 +6843,7 @@
         <v>20</v>
       </c>
       <c r="H113" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="I113" t="s">
         <v>22</v>
@@ -6873,19 +6864,19 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B114" t="s">
         <v>15</v>
       </c>
       <c r="C114" t="s">
-        <v>229</v>
+        <v>152</v>
       </c>
       <c r="D114" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E114" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F114" t="s">
         <v>19</v>
@@ -6894,7 +6885,7 @@
         <v>20</v>
       </c>
       <c r="H114" t="s">
-        <v>469</v>
+        <v>155</v>
       </c>
       <c r="I114" t="s">
         <v>22</v>
@@ -6921,7 +6912,7 @@
         <v>15</v>
       </c>
       <c r="C115" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D115" t="s">
         <v>471</v>
@@ -6936,7 +6927,7 @@
         <v>20</v>
       </c>
       <c r="H115" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I115" t="s">
         <v>22</v>
@@ -6963,7 +6954,7 @@
         <v>15</v>
       </c>
       <c r="C116" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="D116" t="s">
         <v>474</v>
@@ -6978,7 +6969,7 @@
         <v>20</v>
       </c>
       <c r="H116" t="s">
-        <v>158</v>
+        <v>476</v>
       </c>
       <c r="I116" t="s">
         <v>22</v>
@@ -6999,19 +6990,19 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B117" t="s">
         <v>15</v>
       </c>
       <c r="C117" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D117" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E117" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F117" t="s">
         <v>19</v>
@@ -7020,7 +7011,7 @@
         <v>20</v>
       </c>
       <c r="H117" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="I117" t="s">
         <v>22</v>
@@ -7041,19 +7032,19 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B118" t="s">
         <v>15</v>
       </c>
       <c r="C118" t="s">
-        <v>134</v>
+        <v>482</v>
       </c>
       <c r="D118" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="E118" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="F118" t="s">
         <v>19</v>
@@ -7062,7 +7053,7 @@
         <v>20</v>
       </c>
       <c r="H118" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="I118" t="s">
         <v>22</v>
@@ -7083,19 +7074,19 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B119" t="s">
         <v>15</v>
       </c>
       <c r="C119" t="s">
-        <v>485</v>
+        <v>126</v>
       </c>
       <c r="D119" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E119" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F119" t="s">
         <v>19</v>
@@ -7104,7 +7095,7 @@
         <v>20</v>
       </c>
       <c r="H119" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="I119" t="s">
         <v>22</v>
@@ -7125,19 +7116,19 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B120" t="s">
         <v>15</v>
       </c>
       <c r="C120" t="s">
-        <v>129</v>
+        <v>482</v>
       </c>
       <c r="D120" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E120" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F120" t="s">
         <v>19</v>
@@ -7146,7 +7137,7 @@
         <v>20</v>
       </c>
       <c r="H120" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="I120" t="s">
         <v>22</v>
@@ -7167,19 +7158,19 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B121" t="s">
         <v>15</v>
       </c>
       <c r="C121" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D121" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E121" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F121" t="s">
         <v>19</v>
@@ -7188,7 +7179,7 @@
         <v>20</v>
       </c>
       <c r="H121" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="I121" t="s">
         <v>22</v>
@@ -7209,19 +7200,19 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B122" t="s">
         <v>15</v>
       </c>
       <c r="C122" t="s">
-        <v>485</v>
+        <v>126</v>
       </c>
       <c r="D122" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E122" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F122" t="s">
         <v>19</v>
@@ -7230,7 +7221,7 @@
         <v>20</v>
       </c>
       <c r="H122" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="I122" t="s">
         <v>22</v>
@@ -7251,28 +7242,28 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
+        <v>502</v>
+      </c>
+      <c r="B123" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" t="s">
+        <v>126</v>
+      </c>
+      <c r="D123" t="s">
+        <v>503</v>
+      </c>
+      <c r="E123" t="s">
+        <v>504</v>
+      </c>
+      <c r="F123" t="s">
+        <v>19</v>
+      </c>
+      <c r="G123" t="s">
+        <v>20</v>
+      </c>
+      <c r="H123" t="s">
         <v>501</v>
-      </c>
-      <c r="B123" t="s">
-        <v>15</v>
-      </c>
-      <c r="C123" t="s">
-        <v>129</v>
-      </c>
-      <c r="D123" t="s">
-        <v>502</v>
-      </c>
-      <c r="E123" t="s">
-        <v>503</v>
-      </c>
-      <c r="F123" t="s">
-        <v>19</v>
-      </c>
-      <c r="G123" t="s">
-        <v>20</v>
-      </c>
-      <c r="H123" t="s">
-        <v>504</v>
       </c>
       <c r="I123" t="s">
         <v>22</v>
@@ -7299,7 +7290,7 @@
         <v>15</v>
       </c>
       <c r="C124" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D124" t="s">
         <v>506</v>
@@ -7314,7 +7305,7 @@
         <v>20</v>
       </c>
       <c r="H124" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="I124" t="s">
         <v>22</v>
@@ -7335,19 +7326,19 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B125" t="s">
         <v>15</v>
       </c>
       <c r="C125" t="s">
-        <v>134</v>
+        <v>510</v>
       </c>
       <c r="D125" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E125" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="F125" t="s">
         <v>19</v>
@@ -7356,7 +7347,7 @@
         <v>20</v>
       </c>
       <c r="H125" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="I125" t="s">
         <v>22</v>
@@ -7377,19 +7368,19 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B126" t="s">
         <v>15</v>
       </c>
       <c r="C126" t="s">
-        <v>513</v>
+        <v>141</v>
       </c>
       <c r="D126" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E126" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="F126" t="s">
         <v>19</v>
@@ -7398,7 +7389,7 @@
         <v>20</v>
       </c>
       <c r="H126" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="I126" t="s">
         <v>22</v>
@@ -7419,19 +7410,19 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B127" t="s">
         <v>15</v>
       </c>
       <c r="C127" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D127" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E127" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F127" t="s">
         <v>19</v>
@@ -7440,7 +7431,7 @@
         <v>20</v>
       </c>
       <c r="H127" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="I127" t="s">
         <v>22</v>
@@ -7461,19 +7452,19 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B128" t="s">
         <v>15</v>
       </c>
       <c r="C128" t="s">
-        <v>144</v>
+        <v>523</v>
       </c>
       <c r="D128" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E128" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F128" t="s">
         <v>19</v>
@@ -7482,7 +7473,7 @@
         <v>20</v>
       </c>
       <c r="H128" t="s">
-        <v>524</v>
+        <v>387</v>
       </c>
       <c r="I128" t="s">
         <v>22</v>
@@ -7503,13 +7494,13 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B129" t="s">
         <v>15</v>
       </c>
       <c r="C129" t="s">
-        <v>526</v>
+        <v>482</v>
       </c>
       <c r="D129" t="s">
         <v>527</v>
@@ -7524,7 +7515,7 @@
         <v>20</v>
       </c>
       <c r="H129" t="s">
-        <v>390</v>
+        <v>493</v>
       </c>
       <c r="I129" t="s">
         <v>22</v>
@@ -7551,7 +7542,7 @@
         <v>15</v>
       </c>
       <c r="C130" t="s">
-        <v>485</v>
+        <v>523</v>
       </c>
       <c r="D130" t="s">
         <v>530</v>
@@ -7566,7 +7557,7 @@
         <v>20</v>
       </c>
       <c r="H130" t="s">
-        <v>496</v>
+        <v>532</v>
       </c>
       <c r="I130" t="s">
         <v>22</v>
@@ -7587,19 +7578,19 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B131" t="s">
         <v>15</v>
       </c>
       <c r="C131" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D131" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E131" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="F131" t="s">
         <v>19</v>
@@ -7608,7 +7599,7 @@
         <v>20</v>
       </c>
       <c r="H131" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="I131" t="s">
         <v>22</v>
@@ -7629,19 +7620,19 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B132" t="s">
         <v>15</v>
       </c>
       <c r="C132" t="s">
-        <v>526</v>
+        <v>136</v>
       </c>
       <c r="D132" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E132" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F132" t="s">
         <v>19</v>
@@ -7650,7 +7641,7 @@
         <v>20</v>
       </c>
       <c r="H132" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I132" t="s">
         <v>22</v>
@@ -7671,19 +7662,19 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B133" t="s">
         <v>15</v>
       </c>
       <c r="C133" t="s">
-        <v>139</v>
+        <v>542</v>
       </c>
       <c r="D133" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="E133" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="F133" t="s">
         <v>19</v>
@@ -7692,7 +7683,7 @@
         <v>20</v>
       </c>
       <c r="H133" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="I133" t="s">
         <v>22</v>
@@ -7713,19 +7704,19 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B134" t="s">
         <v>15</v>
       </c>
       <c r="C134" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
       <c r="D134" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E134" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F134" t="s">
         <v>19</v>
@@ -7734,7 +7725,7 @@
         <v>20</v>
       </c>
       <c r="H134" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="I134" t="s">
         <v>22</v>
@@ -7761,7 +7752,7 @@
         <v>15</v>
       </c>
       <c r="C135" t="s">
-        <v>526</v>
+        <v>136</v>
       </c>
       <c r="D135" t="s">
         <v>550</v>
@@ -7776,7 +7767,7 @@
         <v>20</v>
       </c>
       <c r="H135" t="s">
-        <v>539</v>
+        <v>552</v>
       </c>
       <c r="I135" t="s">
         <v>22</v>
@@ -7797,19 +7788,19 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B136" t="s">
         <v>15</v>
       </c>
       <c r="C136" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D136" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E136" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="F136" t="s">
         <v>19</v>
@@ -7818,7 +7809,7 @@
         <v>20</v>
       </c>
       <c r="H136" t="s">
-        <v>555</v>
+        <v>493</v>
       </c>
       <c r="I136" t="s">
         <v>22</v>
@@ -7845,7 +7836,7 @@
         <v>15</v>
       </c>
       <c r="C137" t="s">
-        <v>129</v>
+        <v>482</v>
       </c>
       <c r="D137" t="s">
         <v>557</v>
@@ -7860,7 +7851,7 @@
         <v>20</v>
       </c>
       <c r="H137" t="s">
-        <v>496</v>
+        <v>559</v>
       </c>
       <c r="I137" t="s">
         <v>22</v>
@@ -7881,19 +7872,19 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B138" t="s">
         <v>15</v>
       </c>
       <c r="C138" t="s">
-        <v>485</v>
+        <v>126</v>
       </c>
       <c r="D138" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E138" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F138" t="s">
         <v>19</v>
@@ -7902,7 +7893,7 @@
         <v>20</v>
       </c>
       <c r="H138" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="I138" t="s">
         <v>22</v>
@@ -7923,19 +7914,19 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B139" t="s">
         <v>15</v>
       </c>
       <c r="C139" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D139" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E139" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F139" t="s">
         <v>19</v>
@@ -7944,7 +7935,7 @@
         <v>20</v>
       </c>
       <c r="H139" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="I139" t="s">
         <v>22</v>
@@ -7960,48 +7951,6 @@
       </c>
       <c r="M139" s="2"/>
       <c r="N139" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="s">
-        <v>567</v>
-      </c>
-      <c r="B140" t="s">
-        <v>15</v>
-      </c>
-      <c r="C140" t="s">
-        <v>129</v>
-      </c>
-      <c r="D140" t="s">
-        <v>568</v>
-      </c>
-      <c r="E140" t="s">
-        <v>569</v>
-      </c>
-      <c r="F140" t="s">
-        <v>19</v>
-      </c>
-      <c r="G140" t="s">
-        <v>20</v>
-      </c>
-      <c r="H140" t="s">
-        <v>570</v>
-      </c>
-      <c r="I140" t="s">
-        <v>22</v>
-      </c>
-      <c r="J140" t="s">
-        <v>23</v>
-      </c>
-      <c r="K140" t="s">
-        <v>24</v>
-      </c>
-      <c r="L140" t="s">
-        <v>25</v>
-      </c>
-      <c r="M140" s="2"/>
-      <c r="N140" t="s">
         <v>26</v>
       </c>
     </row>
@@ -8021,10 +7970,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="2">
@@ -8032,7 +7981,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="3">
@@ -8040,7 +7989,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="4">
@@ -8048,7 +7997,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5">
@@ -8056,7 +8005,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="6">
@@ -8064,7 +8013,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7">
@@ -8072,7 +8021,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="8">
@@ -8080,7 +8029,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="9">
@@ -8088,7 +8037,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="10">
@@ -8096,7 +8045,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="11">
@@ -8104,7 +8053,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="12">
@@ -8112,7 +8061,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="13">
@@ -8120,7 +8069,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="14">
@@ -8128,7 +8077,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="15">
@@ -8136,7 +8085,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>